<commit_message>
Add 2WLS design, terminal blocks for ground banana
New board 2WLS-30W for The Beast UK two space boat. Also add terminal blocks for ground bananas on Buchla format 30W and 40W boards. Correct filename on OTHER BOM.
</commit_message>
<xml_diff>
--- a/6WLS-30W-BOM.xlsx
+++ b/6WLS-30W-BOM.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Qty</t>
   </si>
@@ -154,9 +154,6 @@
     <t>5V DCDC Converter</t>
   </si>
   <si>
-    <t>DCDCMULT7</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -179,6 +176,15 @@
   </si>
   <si>
     <t>POLARIZED ALUM CAPACITOR</t>
+  </si>
+  <si>
+    <t>MKDSN</t>
+  </si>
+  <si>
+    <t>Terminal Block</t>
+  </si>
+  <si>
+    <t>PHOENIX</t>
   </si>
 </sst>
 </file>
@@ -222,9 +228,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,9 +518,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -571,7 +582,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -619,7 +630,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -650,16 +661,16 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
         <v>33</v>
       </c>
       <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
         <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -667,19 +678,19 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>37</v>
-      </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -700,6 +711,26 @@
       </c>
       <c r="F10" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1729128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>